<commit_message>
Data-driven framework (You can use for API as well Selenium)
</commit_message>
<xml_diff>
--- a/ExcelFiles/APITestData.xlsx
+++ b/ExcelFiles/APITestData.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33765" windowHeight="8085" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33765" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="6" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Validation" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Port</t>
   </si>
@@ -68,24 +69,6 @@
     <t>ApiTest1</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>301</t>
-  </si>
-  <si>
-    <t>API-3</t>
-  </si>
-  <si>
-    <t>API-2</t>
-  </si>
-  <si>
-    <t>API-1</t>
-  </si>
-  <si>
-    <t>API-4</t>
-  </si>
-  <si>
     <t>/payments</t>
   </si>
   <si>
@@ -93,13 +76,31 @@
   </si>
   <si>
     <t>/hasan</t>
+  </si>
+  <si>
+    <t>DataID</t>
+  </si>
+  <si>
+    <t>ResponseContentType</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>JSON</t>
+  </si>
+  <si>
+    <t>XML</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,8 +123,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +163,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -167,14 +182,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,10 +530,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,53 +541,50 @@
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>21</v>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
@@ -579,78 +593,126 @@
       <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
+      <c r="B4">
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
+      <c r="B5">
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>22</v>
+      <c r="B6">
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>